<commit_message>
basic changes to aquifer plot. added mcl lines
</commit_message>
<xml_diff>
--- a/Output/Final_Exports/BTEX_Cases_Well_Data.xlsx
+++ b/Output/Final_Exports/BTEX_Cases_Well_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\R_Scripts\BTEX_Study\Output\Final_Exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\R_Scripts\BTEX_VC\Output\Final_Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09D58F1-FE2A-4B93-8989-0529BFEC5763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F952A111-3AB3-447A-BE53-235789947DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,19 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BTEX_Cases!$A$1:$AD$73</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1150,7 +1162,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1542,7 +1556,7 @@
         <v>53</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>173</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -2025,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>2.4</v>
       </c>
       <c r="O11">
         <v>0</v>

</xml_diff>